<commit_message>
Split cytof analysis templates and tests
still a few tests failing
</commit_message>
<xml_diff>
--- a/template_examples/cytof_e4412_template.xlsx
+++ b/template_examples/cytof_e4412_template.xlsx
@@ -1118,10 +1118,10 @@
   <dimension ref="A1:J2011"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -11331,11 +11331,11 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -21476,7 +21476,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -31619,7 +31619,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -32053,7 +32053,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>

</xml_diff>